<commit_message>
changed names of parties colms
</commit_message>
<xml_diff>
--- a/index 2018.xlsx
+++ b/index 2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabi9\Desktop\Dev\python_dev\elections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB40A5C4-9059-44DA-817E-003DDB31E9A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E6955C-8467-45DA-8AEC-E558029DE666}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="רשימת הגליונות בקובץ זה" sheetId="1" r:id="rId1"/>
@@ -3172,6 +3172,33 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" readingOrder="1"/>
     </xf>
@@ -3180,33 +3207,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -3572,7 +3572,7 @@
   <sheetPr codeName="גיליון1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
@@ -4733,8 +4733,8 @@
   <sheetPr codeName="גיליון2"/>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -5636,7 +5636,7 @@
   <dimension ref="B1:F73"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -5648,13 +5648,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" s="10" customFormat="1" ht="17.399999999999999">
-      <c r="B1" s="236" t="s">
+      <c r="B1" s="245" t="s">
         <v>370</v>
       </c>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
     </row>
     <row r="2" spans="2:6" s="10" customFormat="1" ht="16.2" thickBot="1">
       <c r="B2" s="18"/>
@@ -5685,8 +5685,8 @@
       <c r="C4" s="99" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="237"/>
-      <c r="E4" s="243" t="s">
+      <c r="D4" s="246"/>
+      <c r="E4" s="240" t="s">
         <v>160</v>
       </c>
       <c r="F4" s="100">
@@ -5698,8 +5698,8 @@
       <c r="C5" s="102" t="s">
         <v>164</v>
       </c>
-      <c r="D5" s="238"/>
-      <c r="E5" s="244"/>
+      <c r="D5" s="247"/>
+      <c r="E5" s="241"/>
       <c r="F5" s="103">
         <v>112</v>
       </c>
@@ -5709,10 +5709,10 @@
       <c r="C6" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="239" t="s">
+      <c r="D6" s="236" t="s">
         <v>169</v>
       </c>
-      <c r="E6" s="245" t="s">
+      <c r="E6" s="242" t="s">
         <v>167</v>
       </c>
       <c r="F6" s="103">
@@ -5724,8 +5724,8 @@
       <c r="C7" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="D7" s="240"/>
-      <c r="E7" s="246"/>
+      <c r="D7" s="237"/>
+      <c r="E7" s="243"/>
       <c r="F7" s="103">
         <v>212</v>
       </c>
@@ -5735,8 +5735,8 @@
       <c r="C8" s="102" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="240"/>
-      <c r="E8" s="246"/>
+      <c r="D8" s="237"/>
+      <c r="E8" s="243"/>
       <c r="F8" s="103">
         <v>213</v>
       </c>
@@ -5748,8 +5748,8 @@
       <c r="C9" s="226" t="s">
         <v>551</v>
       </c>
-      <c r="D9" s="241"/>
-      <c r="E9" s="246"/>
+      <c r="D9" s="238"/>
+      <c r="E9" s="243"/>
       <c r="F9" s="225">
         <v>214</v>
       </c>
@@ -5759,10 +5759,10 @@
       <c r="C10" s="102" t="s">
         <v>177</v>
       </c>
-      <c r="D10" s="239" t="s">
+      <c r="D10" s="236" t="s">
         <v>175</v>
       </c>
-      <c r="E10" s="246"/>
+      <c r="E10" s="243"/>
       <c r="F10" s="103">
         <v>221</v>
       </c>
@@ -5772,8 +5772,8 @@
       <c r="C11" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="241"/>
-      <c r="E11" s="246"/>
+      <c r="D11" s="238"/>
+      <c r="E11" s="243"/>
       <c r="F11" s="103">
         <v>222</v>
       </c>
@@ -5783,10 +5783,10 @@
       <c r="C12" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="D12" s="239" t="s">
+      <c r="D12" s="236" t="s">
         <v>181</v>
       </c>
-      <c r="E12" s="246"/>
+      <c r="E12" s="243"/>
       <c r="F12" s="103">
         <v>231</v>
       </c>
@@ -5796,8 +5796,8 @@
       <c r="C13" s="102" t="s">
         <v>184</v>
       </c>
-      <c r="D13" s="240"/>
-      <c r="E13" s="246"/>
+      <c r="D13" s="237"/>
+      <c r="E13" s="243"/>
       <c r="F13" s="103">
         <v>232</v>
       </c>
@@ -5807,8 +5807,8 @@
       <c r="C14" s="102" t="s">
         <v>186</v>
       </c>
-      <c r="D14" s="240"/>
-      <c r="E14" s="246"/>
+      <c r="D14" s="237"/>
+      <c r="E14" s="243"/>
       <c r="F14" s="103">
         <v>233</v>
       </c>
@@ -5818,8 +5818,8 @@
       <c r="C15" s="102" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="240"/>
-      <c r="E15" s="246"/>
+      <c r="D15" s="237"/>
+      <c r="E15" s="243"/>
       <c r="F15" s="103">
         <v>234</v>
       </c>
@@ -5829,8 +5829,8 @@
       <c r="C16" s="102" t="s">
         <v>189</v>
       </c>
-      <c r="D16" s="240"/>
-      <c r="E16" s="246"/>
+      <c r="D16" s="237"/>
+      <c r="E16" s="243"/>
       <c r="F16" s="103">
         <v>235</v>
       </c>
@@ -5840,8 +5840,8 @@
       <c r="C17" s="102" t="s">
         <v>191</v>
       </c>
-      <c r="D17" s="240"/>
-      <c r="E17" s="246"/>
+      <c r="D17" s="237"/>
+      <c r="E17" s="243"/>
       <c r="F17" s="103">
         <v>236</v>
       </c>
@@ -5851,8 +5851,8 @@
       <c r="C18" s="102" t="s">
         <v>192</v>
       </c>
-      <c r="D18" s="241"/>
-      <c r="E18" s="246"/>
+      <c r="D18" s="238"/>
+      <c r="E18" s="243"/>
       <c r="F18" s="103">
         <v>237</v>
       </c>
@@ -5862,10 +5862,10 @@
       <c r="C19" s="102" t="s">
         <v>196</v>
       </c>
-      <c r="D19" s="239" t="s">
+      <c r="D19" s="236" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="246"/>
+      <c r="E19" s="243"/>
       <c r="F19" s="103">
         <v>241</v>
       </c>
@@ -5875,8 +5875,8 @@
       <c r="C20" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="D20" s="240"/>
-      <c r="E20" s="246"/>
+      <c r="D20" s="237"/>
+      <c r="E20" s="243"/>
       <c r="F20" s="103">
         <v>242</v>
       </c>
@@ -5886,8 +5886,8 @@
       <c r="C21" s="102" t="s">
         <v>200</v>
       </c>
-      <c r="D21" s="240"/>
-      <c r="E21" s="246"/>
+      <c r="D21" s="237"/>
+      <c r="E21" s="243"/>
       <c r="F21" s="103">
         <v>243</v>
       </c>
@@ -5897,8 +5897,8 @@
       <c r="C22" s="102" t="s">
         <v>202</v>
       </c>
-      <c r="D22" s="240"/>
-      <c r="E22" s="246"/>
+      <c r="D22" s="237"/>
+      <c r="E22" s="243"/>
       <c r="F22" s="103">
         <v>244</v>
       </c>
@@ -5908,8 +5908,8 @@
       <c r="C23" s="102" t="s">
         <v>204</v>
       </c>
-      <c r="D23" s="240"/>
-      <c r="E23" s="246"/>
+      <c r="D23" s="237"/>
+      <c r="E23" s="243"/>
       <c r="F23" s="103">
         <v>245</v>
       </c>
@@ -5919,8 +5919,8 @@
       <c r="C24" s="102" t="s">
         <v>206</v>
       </c>
-      <c r="D24" s="241"/>
-      <c r="E24" s="246"/>
+      <c r="D24" s="238"/>
+      <c r="E24" s="243"/>
       <c r="F24" s="103">
         <v>246</v>
       </c>
@@ -5930,10 +5930,10 @@
       <c r="C25" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="D25" s="239" t="s">
+      <c r="D25" s="236" t="s">
         <v>208</v>
       </c>
-      <c r="E25" s="246"/>
+      <c r="E25" s="243"/>
       <c r="F25" s="103">
         <v>291</v>
       </c>
@@ -5943,8 +5943,8 @@
       <c r="C26" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="D26" s="240"/>
-      <c r="E26" s="246"/>
+      <c r="D26" s="237"/>
+      <c r="E26" s="243"/>
       <c r="F26" s="103">
         <v>292</v>
       </c>
@@ -5954,8 +5954,8 @@
       <c r="C27" s="102" t="s">
         <v>214</v>
       </c>
-      <c r="D27" s="240"/>
-      <c r="E27" s="246"/>
+      <c r="D27" s="237"/>
+      <c r="E27" s="243"/>
       <c r="F27" s="103">
         <v>293</v>
       </c>
@@ -5965,8 +5965,8 @@
       <c r="C28" s="102" t="s">
         <v>216</v>
       </c>
-      <c r="D28" s="241"/>
-      <c r="E28" s="244"/>
+      <c r="D28" s="238"/>
+      <c r="E28" s="241"/>
       <c r="F28" s="103">
         <v>294</v>
       </c>
@@ -5979,7 +5979,7 @@
       <c r="D29" s="104" t="s">
         <v>220</v>
       </c>
-      <c r="E29" s="245" t="s">
+      <c r="E29" s="242" t="s">
         <v>219</v>
       </c>
       <c r="F29" s="103">
@@ -5991,10 +5991,10 @@
       <c r="C30" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="239" t="s">
+      <c r="D30" s="236" t="s">
         <v>222</v>
       </c>
-      <c r="E30" s="246"/>
+      <c r="E30" s="243"/>
       <c r="F30" s="103">
         <v>321</v>
       </c>
@@ -6004,8 +6004,8 @@
       <c r="C31" s="102" t="s">
         <v>223</v>
       </c>
-      <c r="D31" s="240"/>
-      <c r="E31" s="246"/>
+      <c r="D31" s="237"/>
+      <c r="E31" s="243"/>
       <c r="F31" s="103">
         <v>322</v>
       </c>
@@ -6015,8 +6015,8 @@
       <c r="C32" s="102" t="s">
         <v>224</v>
       </c>
-      <c r="D32" s="240"/>
-      <c r="E32" s="246"/>
+      <c r="D32" s="237"/>
+      <c r="E32" s="243"/>
       <c r="F32" s="103">
         <v>323</v>
       </c>
@@ -6026,8 +6026,8 @@
       <c r="C33" s="102" t="s">
         <v>225</v>
       </c>
-      <c r="D33" s="241"/>
-      <c r="E33" s="244"/>
+      <c r="D33" s="238"/>
+      <c r="E33" s="241"/>
       <c r="F33" s="103">
         <v>324</v>
       </c>
@@ -6037,10 +6037,10 @@
       <c r="C34" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="D34" s="239" t="s">
+      <c r="D34" s="236" t="s">
         <v>163</v>
       </c>
-      <c r="E34" s="245" t="s">
+      <c r="E34" s="242" t="s">
         <v>161</v>
       </c>
       <c r="F34" s="106">
@@ -6052,8 +6052,8 @@
       <c r="C35" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="D35" s="241"/>
-      <c r="E35" s="246"/>
+      <c r="D35" s="238"/>
+      <c r="E35" s="243"/>
       <c r="F35" s="106">
         <v>412</v>
       </c>
@@ -6063,10 +6063,10 @@
       <c r="C36" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="239" t="s">
+      <c r="D36" s="236" t="s">
         <v>168</v>
       </c>
-      <c r="E36" s="246"/>
+      <c r="E36" s="243"/>
       <c r="F36" s="106">
         <v>421</v>
       </c>
@@ -6076,8 +6076,8 @@
       <c r="C37" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="D37" s="241"/>
-      <c r="E37" s="246"/>
+      <c r="D37" s="238"/>
+      <c r="E37" s="243"/>
       <c r="F37" s="106">
         <v>422</v>
       </c>
@@ -6090,7 +6090,7 @@
       <c r="D38" s="104" t="s">
         <v>173</v>
       </c>
-      <c r="E38" s="246"/>
+      <c r="E38" s="243"/>
       <c r="F38" s="106">
         <v>431</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>443</v>
       </c>
       <c r="D39" s="104"/>
-      <c r="E39" s="246"/>
+      <c r="E39" s="243"/>
       <c r="F39" s="106">
         <v>432</v>
       </c>
@@ -6111,10 +6111,10 @@
       <c r="C40" s="102" t="s">
         <v>178</v>
       </c>
-      <c r="D40" s="239" t="s">
+      <c r="D40" s="236" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="246"/>
+      <c r="E40" s="243"/>
       <c r="F40" s="106">
         <v>441</v>
       </c>
@@ -6124,8 +6124,8 @@
       <c r="C41" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="241"/>
-      <c r="E41" s="244"/>
+      <c r="D41" s="238"/>
+      <c r="E41" s="241"/>
       <c r="F41" s="106">
         <v>442</v>
       </c>
@@ -6135,10 +6135,10 @@
       <c r="C42" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="D42" s="239" t="s">
+      <c r="D42" s="236" t="s">
         <v>185</v>
       </c>
-      <c r="E42" s="245" t="s">
+      <c r="E42" s="242" t="s">
         <v>183</v>
       </c>
       <c r="F42" s="106">
@@ -6150,8 +6150,8 @@
       <c r="C43" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="D43" s="240"/>
-      <c r="E43" s="246"/>
+      <c r="D43" s="237"/>
+      <c r="E43" s="243"/>
       <c r="F43" s="106">
         <v>512</v>
       </c>
@@ -6161,8 +6161,8 @@
       <c r="C44" s="102" t="s">
         <v>190</v>
       </c>
-      <c r="D44" s="241"/>
-      <c r="E44" s="244"/>
+      <c r="D44" s="238"/>
+      <c r="E44" s="241"/>
       <c r="F44" s="106">
         <v>513</v>
       </c>
@@ -6172,10 +6172,10 @@
       <c r="C45" s="102" t="s">
         <v>197</v>
       </c>
-      <c r="D45" s="239" t="s">
+      <c r="D45" s="236" t="s">
         <v>195</v>
       </c>
-      <c r="E45" s="245" t="s">
+      <c r="E45" s="242" t="s">
         <v>193</v>
       </c>
       <c r="F45" s="106">
@@ -6187,8 +6187,8 @@
       <c r="C46" s="102" t="s">
         <v>199</v>
       </c>
-      <c r="D46" s="240"/>
-      <c r="E46" s="246"/>
+      <c r="D46" s="237"/>
+      <c r="E46" s="243"/>
       <c r="F46" s="106">
         <v>612</v>
       </c>
@@ -6198,8 +6198,8 @@
       <c r="C47" s="102" t="s">
         <v>201</v>
       </c>
-      <c r="D47" s="240"/>
-      <c r="E47" s="246"/>
+      <c r="D47" s="237"/>
+      <c r="E47" s="243"/>
       <c r="F47" s="106">
         <v>613</v>
       </c>
@@ -6209,8 +6209,8 @@
       <c r="C48" s="102" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="241"/>
-      <c r="E48" s="246"/>
+      <c r="D48" s="238"/>
+      <c r="E48" s="243"/>
       <c r="F48" s="106">
         <v>614</v>
       </c>
@@ -6220,10 +6220,10 @@
       <c r="C49" s="102" t="s">
         <v>207</v>
       </c>
-      <c r="D49" s="239" t="s">
+      <c r="D49" s="236" t="s">
         <v>205</v>
       </c>
-      <c r="E49" s="246"/>
+      <c r="E49" s="243"/>
       <c r="F49" s="106">
         <v>621</v>
       </c>
@@ -6233,8 +6233,8 @@
       <c r="C50" s="102" t="s">
         <v>209</v>
       </c>
-      <c r="D50" s="240"/>
-      <c r="E50" s="246"/>
+      <c r="D50" s="237"/>
+      <c r="E50" s="243"/>
       <c r="F50" s="106">
         <v>622</v>
       </c>
@@ -6244,8 +6244,8 @@
       <c r="C51" s="102" t="s">
         <v>211</v>
       </c>
-      <c r="D51" s="240"/>
-      <c r="E51" s="246"/>
+      <c r="D51" s="237"/>
+      <c r="E51" s="243"/>
       <c r="F51" s="106">
         <v>623</v>
       </c>
@@ -6255,8 +6255,8 @@
       <c r="C52" s="102" t="s">
         <v>213</v>
       </c>
-      <c r="D52" s="240"/>
-      <c r="E52" s="246"/>
+      <c r="D52" s="237"/>
+      <c r="E52" s="243"/>
       <c r="F52" s="106">
         <v>624</v>
       </c>
@@ -6266,8 +6266,8 @@
       <c r="C53" s="102" t="s">
         <v>215</v>
       </c>
-      <c r="D53" s="240"/>
-      <c r="E53" s="246"/>
+      <c r="D53" s="237"/>
+      <c r="E53" s="243"/>
       <c r="F53" s="106">
         <v>625</v>
       </c>
@@ -6277,8 +6277,8 @@
       <c r="C54" s="102" t="s">
         <v>217</v>
       </c>
-      <c r="D54" s="240"/>
-      <c r="E54" s="246"/>
+      <c r="D54" s="237"/>
+      <c r="E54" s="243"/>
       <c r="F54" s="106">
         <v>626</v>
       </c>
@@ -6288,8 +6288,8 @@
       <c r="C55" s="108" t="s">
         <v>218</v>
       </c>
-      <c r="D55" s="242"/>
-      <c r="E55" s="247"/>
+      <c r="D55" s="239"/>
+      <c r="E55" s="244"/>
       <c r="F55" s="109">
         <v>627</v>
       </c>
@@ -6394,6 +6394,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D40:D41"/>
     <mergeCell ref="D45:D48"/>
     <mergeCell ref="D49:D55"/>
     <mergeCell ref="E4:E5"/>
@@ -6409,11 +6414,6 @@
     <mergeCell ref="D19:D24"/>
     <mergeCell ref="D25:D28"/>
     <mergeCell ref="D30:D33"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D40:D41"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6431,7 +6431,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -8778,62 +8778,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CbsHide xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
-    <PublishingRollupImage xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <CbsPublishingDocSubjectEng xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
-    <ArticleStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3">2019-09-24T21:00:00+00:00</ArticleStartDate>
-    <eWaveListOrderValue xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <CbsPublishingDocSubject xmlns="f37fff55-d014-472b-b062-823f736a4040">יישובים בישראל- קובצי יישובים, 2018-2003</CbsPublishingDocSubject>
-    <CbsDocArticleVariationRelUrlEng xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
-    <CbsPublishingDocChapterEng xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
-    <CbsPublishingDocChapter xmlns="f37fff55-d014-472b-b062-823f736a4040">ביאור סמלי החלוקות הגאוגרפיות</CbsPublishingDocChapter>
-    <CbsDataSource xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <VariationsItemGroupID xmlns="http://schemas.microsoft.com/sharepoint/v3">b413cf99-8ead-45f5-878a-df1a5ab4292c</VariationsItemGroupID>
-    <CbsOrderField xmlns="f37fff55-d014-472b-b062-823f736a4040">18</CbsOrderField>
-    <CbsEnglishTitle xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
-    <badce114fb994f27a777030e336d1efa xmlns="f37fff55-d014-472b-b062-823f736a4040">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">תפרוסת גאוגרפית</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">42494796-41ed-4e4a-95c2-c33df452209e</TermId>
-        </TermInfo>
-      </Terms>
-    </badce114fb994f27a777030e336d1efa>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-    <CbsMadadPublishDate xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
-    <CbsDocArticleVariationRelUrl xmlns="f37fff55-d014-472b-b062-823f736a4040">/he/publications/Pages/2019/יישובים-בישראל.aspx</CbsDocArticleVariationRelUrl>
-    <CbsDataPublishDate xmlns="f37fff55-d014-472b-b062-823f736a4040">2019-09-01T10:00:00+00:00</CbsDataPublishDate>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך פרסום למס" ma:contentTypeID="0x01010018C65C5FFA1A411CB733A36D5E05D176005EC8771B28134F43A3AE7296363CCDAA00776BC5533B746B4DA895265925393F0F" ma:contentTypeVersion="71" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="282a9a53f14a8d9affd9cb22076dd0d9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f37fff55-d014-472b-b062-823f736a4040" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d805af3f622143f99170ddeddda7902" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9126,32 +9070,63 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F126064-31F9-44E6-A033-D58D8EC74FEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f37fff55-d014-472b-b062-823f736a4040"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF146A5A-D861-41F9-9D5A-CA972868EBB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CbsHide xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
+    <PublishingRollupImage xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <CbsPublishingDocSubjectEng xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
+    <ArticleStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3">2019-09-24T21:00:00+00:00</ArticleStartDate>
+    <eWaveListOrderValue xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <CbsPublishingDocSubject xmlns="f37fff55-d014-472b-b062-823f736a4040">יישובים בישראל- קובצי יישובים, 2018-2003</CbsPublishingDocSubject>
+    <CbsDocArticleVariationRelUrlEng xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
+    <CbsPublishingDocChapterEng xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
+    <CbsPublishingDocChapter xmlns="f37fff55-d014-472b-b062-823f736a4040">ביאור סמלי החלוקות הגאוגרפיות</CbsPublishingDocChapter>
+    <CbsDataSource xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <VariationsItemGroupID xmlns="http://schemas.microsoft.com/sharepoint/v3">b413cf99-8ead-45f5-878a-df1a5ab4292c</VariationsItemGroupID>
+    <CbsOrderField xmlns="f37fff55-d014-472b-b062-823f736a4040">18</CbsOrderField>
+    <CbsEnglishTitle xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
+    <badce114fb994f27a777030e336d1efa xmlns="f37fff55-d014-472b-b062-823f736a4040">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">תפרוסת גאוגרפית</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">42494796-41ed-4e4a-95c2-c33df452209e</TermId>
+        </TermInfo>
+      </Terms>
+    </badce114fb994f27a777030e336d1efa>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+    <CbsMadadPublishDate xmlns="f37fff55-d014-472b-b062-823f736a4040" xsi:nil="true"/>
+    <CbsDocArticleVariationRelUrl xmlns="f37fff55-d014-472b-b062-823f736a4040">/he/publications/Pages/2019/יישובים-בישראל.aspx</CbsDocArticleVariationRelUrl>
+    <CbsDataPublishDate xmlns="f37fff55-d014-472b-b062-823f736a4040">2019-09-01T10:00:00+00:00</CbsDataPublishDate>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8708237-B15E-4990-BA8C-DC81E8D306CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9168,4 +9143,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF146A5A-D861-41F9-9D5A-CA972868EBB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F126064-31F9-44E6-A033-D58D8EC74FEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f37fff55-d014-472b-b062-823f736a4040"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>